<commit_message>
convert meter to degree by brute force method
</commit_message>
<xml_diff>
--- a/Data/cctv_locations_master - Copy.xlsx
+++ b/Data/cctv_locations_master - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naris\Desktop\STIU\2024-1 Internship\Gistda\2024-07-01 Image Scraping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F511DE-D78A-4C26-8932-93A1F08CCB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0FCF14-9603-48AF-A7F0-3F7F235441F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5768" uniqueCount="3514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6025" uniqueCount="3642">
   <si>
     <t>ID</t>
   </si>
@@ -10575,6 +10575,390 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>1638</t>
+  </si>
+  <si>
+    <t>10.140.116.89</t>
+  </si>
+  <si>
+    <t>1231</t>
+  </si>
+  <si>
+    <t>DS-31-05</t>
+  </si>
+  <si>
+    <t>10.102.101.163</t>
+  </si>
+  <si>
+    <t>1423</t>
+  </si>
+  <si>
+    <t>10.101.102.69</t>
+  </si>
+  <si>
+    <t>1418</t>
+  </si>
+  <si>
+    <t>PN-29-01</t>
+  </si>
+  <si>
+    <t>แยกเฉลิมไทย</t>
+  </si>
+  <si>
+    <t>10.101.102.77</t>
+  </si>
+  <si>
+    <t>1755</t>
+  </si>
+  <si>
+    <t>PT-08-02-03</t>
+  </si>
+  <si>
+    <t>Pathum Wan Intersection</t>
+  </si>
+  <si>
+    <t>แยกปทุมวัน</t>
+  </si>
+  <si>
+    <t>10.107.101.62</t>
+  </si>
+  <si>
+    <t>1282</t>
+  </si>
+  <si>
+    <t>TF1-HK-02</t>
+  </si>
+  <si>
+    <t>ถนนพระราม 9 ตัด ถนนตัดใหม่</t>
+  </si>
+  <si>
+    <t>10.156.101.37</t>
+  </si>
+  <si>
+    <t>1287</t>
+  </si>
+  <si>
+    <t>TF1-LK-01</t>
+  </si>
+  <si>
+    <t>ถ.ฉลองกรุง ตัด มอเตอร์เวย์</t>
+  </si>
+  <si>
+    <t>10.156.101.33</t>
+  </si>
+  <si>
+    <t>1247</t>
+  </si>
+  <si>
+    <t>TF1-LS-02</t>
+  </si>
+  <si>
+    <t>ถ.แจ้งวัฒนะ ตัด ถ.เลียบคลองประปา</t>
+  </si>
+  <si>
+    <t>10.156.101.22</t>
+  </si>
+  <si>
+    <t>1641</t>
+  </si>
+  <si>
+    <t>TF-DD-01</t>
+  </si>
+  <si>
+    <t>แยกดินแดง</t>
+  </si>
+  <si>
+    <t>10.156.102.1</t>
+  </si>
+  <si>
+    <t>1166</t>
+  </si>
+  <si>
+    <t>TF-HW-01-02-17</t>
+  </si>
+  <si>
+    <t>ทางขึ้นสะพานพระราม8</t>
+  </si>
+  <si>
+    <t>TF-HW-01-02-17 ทางขึ้นสะพานพระราม8	ขาเข้า</t>
+  </si>
+  <si>
+    <t>10.151.101.37</t>
+  </si>
+  <si>
+    <t>1167</t>
+  </si>
+  <si>
+    <t>TF-HW-01-02-18</t>
+  </si>
+  <si>
+    <t>TF-HW-01-02-18 ทางขึ้นสะพานพระราม 8</t>
+  </si>
+  <si>
+    <t>10.151.101.38</t>
+  </si>
+  <si>
+    <t>289</t>
+  </si>
+  <si>
+    <t>TF-HW-01-02-25</t>
+  </si>
+  <si>
+    <t>ช่วงแยกบรมราชชนนี</t>
+  </si>
+  <si>
+    <t>10.151.101.45</t>
+  </si>
+  <si>
+    <t>1649</t>
+  </si>
+  <si>
+    <t>TF-PN-02</t>
+  </si>
+  <si>
+    <t>หลักเมือง</t>
+  </si>
+  <si>
+    <t>10.156.102.11</t>
+  </si>
+  <si>
+    <t>1650</t>
+  </si>
+  <si>
+    <t>TF-PN-03</t>
+  </si>
+  <si>
+    <t>ป้อมมหากาฬ</t>
+  </si>
+  <si>
+    <t>10.156.102.12</t>
+  </si>
+  <si>
+    <t>1672</t>
+  </si>
+  <si>
+    <t>TF-WT-02</t>
+  </si>
+  <si>
+    <t>คลองบางกะปิ</t>
+  </si>
+  <si>
+    <t>10.156.102.83</t>
+  </si>
+  <si>
+    <t>1677</t>
+  </si>
+  <si>
+    <t>10.147.116.25</t>
+  </si>
+  <si>
+    <t>1678</t>
+  </si>
+  <si>
+    <t>10.147.116.26</t>
+  </si>
+  <si>
+    <t>1673</t>
+  </si>
+  <si>
+    <t>ถ.พระราม 2 ตัด (หน้าบริเวณโรงพยาบาลบางมด)</t>
+  </si>
+  <si>
+    <t>10.156.101.63</t>
+  </si>
+  <si>
+    <t>1296</t>
+  </si>
+  <si>
+    <t>ถ.รามอินทรา ตรงข้ามปากซอยรามอินทรา 39</t>
+  </si>
+  <si>
+    <t>10.156.101.17</t>
+  </si>
+  <si>
+    <t>1751</t>
+  </si>
+  <si>
+    <t>ถ.ลำลูกกา ตัด ถ.พหลโยธิน</t>
+  </si>
+  <si>
+    <t>10.156.101.48</t>
+  </si>
+  <si>
+    <t>1161</t>
+  </si>
+  <si>
+    <t>ทางขึ้น ด่วนยกระดับฝั่งปิ่นเกล้า ขาออก</t>
+  </si>
+  <si>
+    <t>10.151.101.31</t>
+  </si>
+  <si>
+    <t>1163</t>
+  </si>
+  <si>
+    <t>10.151.101.34</t>
+  </si>
+  <si>
+    <t>1164</t>
+  </si>
+  <si>
+    <t>ทางด่วนยกระดับฝั่งปิ่นเกล้า ช่วงทางลงศิริราช	 ขาออก</t>
+  </si>
+  <si>
+    <t>10.151.101.35</t>
+  </si>
+  <si>
+    <t>413</t>
+  </si>
+  <si>
+    <t>แนวถนนตะนาว</t>
+  </si>
+  <si>
+    <t>Tanao Road</t>
+  </si>
+  <si>
+    <t>จากแยกสี่กั๊กเสาชิงช้า มุ่งหน้าแยกคอกวัว</t>
+  </si>
+  <si>
+    <t>From Si Kak Sao Ching Cha Intersection towards Khok Wua Intersection</t>
+  </si>
+  <si>
+    <t>10.101.102.190</t>
+  </si>
+  <si>
+    <t>1503</t>
+  </si>
+  <si>
+    <t>10.101.102.216</t>
+  </si>
+  <si>
+    <t>414</t>
+  </si>
+  <si>
+    <t>บริเวณใต้สะพานพุทธ</t>
+  </si>
+  <si>
+    <t>Below/Under Phra Phuttha Yodfa Bridge (Memorial Bridge)</t>
+  </si>
+  <si>
+    <t>มุ่งหน้ามาปากคลองตลาด</t>
+  </si>
+  <si>
+    <t>Towards Pak Khlong Talat</t>
+  </si>
+  <si>
+    <t>10.101.102.200</t>
+  </si>
+  <si>
+    <t>1506</t>
+  </si>
+  <si>
+    <t>แยกคอกวัว ถนนราชดำเนินกลาง เขตพระนคร</t>
+  </si>
+  <si>
+    <t>แยกคอกวัว ถนนราชดำเนินกลาง</t>
+  </si>
+  <si>
+    <t>10.101.102.30</t>
+  </si>
+  <si>
+    <t>1497</t>
+  </si>
+  <si>
+    <t>10.101.102.71</t>
+  </si>
+  <si>
+    <t>1557</t>
+  </si>
+  <si>
+    <t>10.107.102.26</t>
+  </si>
+  <si>
+    <t>317</t>
+  </si>
+  <si>
+    <t>แยกบรมราชชนนี ด้านถนนจรัญสนิทวงศ์</t>
+  </si>
+  <si>
+    <t>รถมุ่งหน้าไปแยกบางพลัด</t>
+  </si>
+  <si>
+    <t>Towards Lan Phra Rup Intersection</t>
+  </si>
+  <si>
+    <t>10.151.101.43</t>
+  </si>
+  <si>
+    <t>388</t>
+  </si>
+  <si>
+    <t>แยกวิสุทธิกษัตริย์ ด้านถนนประชาธิปไตย</t>
+  </si>
+  <si>
+    <t>รถมุ่งหน้าไปแยกประชาเกษม</t>
+  </si>
+  <si>
+    <t>Left side towards Chalermwanchat Intersection</t>
+  </si>
+  <si>
+    <t>10.101.101.76</t>
+  </si>
+  <si>
+    <t>1397</t>
+  </si>
+  <si>
+    <t>10.101.101.101</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>รถมาจากแยกตากสิน มุ่งหน้าไปแยกมไหสวรรย์</t>
+  </si>
+  <si>
+    <t>From Charoen Nakhon Tai Intersection towards Buk Ka Lo Intersection</t>
+  </si>
+  <si>
+    <t>10.116.129.123</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>หน้า รพ.กลาง ถนนหลวง</t>
+  </si>
+  <si>
+    <t>In front of Klang Hospital on Luang Road</t>
+  </si>
+  <si>
+    <t>รถมาจากแยกโรงพยาบาลกลาง มุ่งหน้าไปแยกวรจักร</t>
+  </si>
+  <si>
+    <t>From Klang Hospital  towards Worachak Intersection</t>
+  </si>
+  <si>
+    <t>10.151.129.124</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>หน้าธนาคารกรุงเทพ สาขาวรจักร ถนนวรจักร</t>
+  </si>
+  <si>
+    <t>In front of bangkokbank Worachak Branch on Worachak Road</t>
+  </si>
+  <si>
+    <t>รถมาจากแยกแม้นศรี มุ่งหน้าไปแยกวรจักร</t>
+  </si>
+  <si>
+    <t>From Worachak Intersection</t>
+  </si>
+  <si>
+    <t>10.151.128.30</t>
   </si>
 </sst>
 </file>
@@ -10989,11 +11373,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N651"/>
+  <dimension ref="A1:N686"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33544,6 +33928,1057 @@
         <v>11</v>
       </c>
     </row>
+    <row r="652" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A652" t="s">
+        <v>3514</v>
+      </c>
+      <c r="B652" t="s">
+        <v>7</v>
+      </c>
+      <c r="E652" t="s">
+        <v>8</v>
+      </c>
+      <c r="G652" t="s">
+        <v>8</v>
+      </c>
+      <c r="I652">
+        <v>13.71186</v>
+      </c>
+      <c r="J652">
+        <v>100.42082000000001</v>
+      </c>
+      <c r="M652" t="s">
+        <v>3515</v>
+      </c>
+      <c r="N652" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="653" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A653" t="s">
+        <v>3516</v>
+      </c>
+      <c r="B653" t="s">
+        <v>3517</v>
+      </c>
+      <c r="E653" t="s">
+        <v>3263</v>
+      </c>
+      <c r="F653" t="s">
+        <v>9</v>
+      </c>
+      <c r="G653" t="s">
+        <v>3263</v>
+      </c>
+      <c r="H653" t="s">
+        <v>9</v>
+      </c>
+      <c r="I653">
+        <v>13.770619999999999</v>
+      </c>
+      <c r="J653">
+        <v>100.526</v>
+      </c>
+      <c r="M653" t="s">
+        <v>3518</v>
+      </c>
+      <c r="N653" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="654" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A654" t="s">
+        <v>3519</v>
+      </c>
+      <c r="B654" t="s">
+        <v>337</v>
+      </c>
+      <c r="E654" t="s">
+        <v>338</v>
+      </c>
+      <c r="F654" t="s">
+        <v>9</v>
+      </c>
+      <c r="G654" t="s">
+        <v>338</v>
+      </c>
+      <c r="H654" t="s">
+        <v>9</v>
+      </c>
+      <c r="I654">
+        <v>13.759969999999999</v>
+      </c>
+      <c r="J654">
+        <v>100.50763000000001</v>
+      </c>
+      <c r="M654" t="s">
+        <v>3520</v>
+      </c>
+      <c r="N654" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="655" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A655" t="s">
+        <v>3521</v>
+      </c>
+      <c r="B655" t="s">
+        <v>3522</v>
+      </c>
+      <c r="E655" t="s">
+        <v>3523</v>
+      </c>
+      <c r="F655" t="s">
+        <v>9</v>
+      </c>
+      <c r="G655" t="s">
+        <v>3523</v>
+      </c>
+      <c r="H655" t="s">
+        <v>9</v>
+      </c>
+      <c r="I655">
+        <v>13.75623</v>
+      </c>
+      <c r="J655">
+        <v>100.5048</v>
+      </c>
+      <c r="M655" t="s">
+        <v>3524</v>
+      </c>
+      <c r="N655" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="656" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A656" t="s">
+        <v>3525</v>
+      </c>
+      <c r="B656" t="s">
+        <v>3526</v>
+      </c>
+      <c r="F656" t="s">
+        <v>3527</v>
+      </c>
+      <c r="G656" t="s">
+        <v>3528</v>
+      </c>
+      <c r="H656" t="s">
+        <v>3527</v>
+      </c>
+      <c r="I656">
+        <v>13.74615</v>
+      </c>
+      <c r="J656">
+        <v>100.53075</v>
+      </c>
+      <c r="M656" t="s">
+        <v>3529</v>
+      </c>
+      <c r="N656" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="657" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A657" t="s">
+        <v>3530</v>
+      </c>
+      <c r="B657" t="s">
+        <v>3531</v>
+      </c>
+      <c r="E657" t="s">
+        <v>3532</v>
+      </c>
+      <c r="F657" t="s">
+        <v>9</v>
+      </c>
+      <c r="G657" t="s">
+        <v>3532</v>
+      </c>
+      <c r="H657" t="s">
+        <v>9</v>
+      </c>
+      <c r="I657">
+        <v>13.74133</v>
+      </c>
+      <c r="J657">
+        <v>100.61593000000001</v>
+      </c>
+      <c r="M657" t="s">
+        <v>3533</v>
+      </c>
+      <c r="N657" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="658" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A658" t="s">
+        <v>3534</v>
+      </c>
+      <c r="B658" t="s">
+        <v>3535</v>
+      </c>
+      <c r="E658" t="s">
+        <v>3536</v>
+      </c>
+      <c r="F658" t="s">
+        <v>9</v>
+      </c>
+      <c r="G658" t="s">
+        <v>3536</v>
+      </c>
+      <c r="H658" t="s">
+        <v>9</v>
+      </c>
+      <c r="I658">
+        <v>13.73268</v>
+      </c>
+      <c r="J658">
+        <v>100.78484</v>
+      </c>
+      <c r="M658" t="s">
+        <v>3537</v>
+      </c>
+      <c r="N658" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="659" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A659" t="s">
+        <v>3538</v>
+      </c>
+      <c r="B659" t="s">
+        <v>3539</v>
+      </c>
+      <c r="E659" t="s">
+        <v>3540</v>
+      </c>
+      <c r="F659" t="s">
+        <v>9</v>
+      </c>
+      <c r="G659" t="s">
+        <v>3540</v>
+      </c>
+      <c r="H659" t="s">
+        <v>9</v>
+      </c>
+      <c r="I659">
+        <v>13.89484</v>
+      </c>
+      <c r="J659">
+        <v>100.55497</v>
+      </c>
+      <c r="M659" t="s">
+        <v>3541</v>
+      </c>
+      <c r="N659" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="660" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A660" t="s">
+        <v>3542</v>
+      </c>
+      <c r="B660" t="s">
+        <v>3543</v>
+      </c>
+      <c r="E660" t="s">
+        <v>3544</v>
+      </c>
+      <c r="F660" t="s">
+        <v>9</v>
+      </c>
+      <c r="G660" t="s">
+        <v>3544</v>
+      </c>
+      <c r="H660" t="s">
+        <v>9</v>
+      </c>
+      <c r="I660">
+        <v>13.76393</v>
+      </c>
+      <c r="J660">
+        <v>100.54785</v>
+      </c>
+      <c r="M660" t="s">
+        <v>3545</v>
+      </c>
+      <c r="N660" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="661" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A661" t="s">
+        <v>3546</v>
+      </c>
+      <c r="B661" t="s">
+        <v>3547</v>
+      </c>
+      <c r="E661" t="s">
+        <v>3548</v>
+      </c>
+      <c r="F661" t="s">
+        <v>9</v>
+      </c>
+      <c r="G661" t="s">
+        <v>3549</v>
+      </c>
+      <c r="H661" t="s">
+        <v>9</v>
+      </c>
+      <c r="I661">
+        <v>13.771660000000001</v>
+      </c>
+      <c r="J661">
+        <v>100.49276</v>
+      </c>
+      <c r="M661" t="s">
+        <v>3550</v>
+      </c>
+      <c r="N661" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="662" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A662" t="s">
+        <v>3551</v>
+      </c>
+      <c r="B662" t="s">
+        <v>3552</v>
+      </c>
+      <c r="E662" t="s">
+        <v>659</v>
+      </c>
+      <c r="F662" t="s">
+        <v>9</v>
+      </c>
+      <c r="G662" t="s">
+        <v>3553</v>
+      </c>
+      <c r="H662" t="s">
+        <v>9</v>
+      </c>
+      <c r="I662">
+        <v>13.771660000000001</v>
+      </c>
+      <c r="J662">
+        <v>100.49276999999999</v>
+      </c>
+      <c r="M662" t="s">
+        <v>3554</v>
+      </c>
+      <c r="N662" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="663" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A663" t="s">
+        <v>3555</v>
+      </c>
+      <c r="B663" t="s">
+        <v>3556</v>
+      </c>
+      <c r="E663" t="s">
+        <v>992</v>
+      </c>
+      <c r="F663" t="s">
+        <v>844</v>
+      </c>
+      <c r="G663" t="s">
+        <v>3557</v>
+      </c>
+      <c r="H663" t="s">
+        <v>846</v>
+      </c>
+      <c r="I663">
+        <v>13.77309</v>
+      </c>
+      <c r="J663">
+        <v>100.48193999999999</v>
+      </c>
+      <c r="M663" t="s">
+        <v>3558</v>
+      </c>
+      <c r="N663" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="664" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A664" t="s">
+        <v>3559</v>
+      </c>
+      <c r="B664" t="s">
+        <v>3560</v>
+      </c>
+      <c r="E664" t="s">
+        <v>3561</v>
+      </c>
+      <c r="F664" t="s">
+        <v>9</v>
+      </c>
+      <c r="G664" t="s">
+        <v>3561</v>
+      </c>
+      <c r="H664" t="s">
+        <v>9</v>
+      </c>
+      <c r="I664">
+        <v>13.75319</v>
+      </c>
+      <c r="J664">
+        <v>100.49373</v>
+      </c>
+      <c r="M664" t="s">
+        <v>3562</v>
+      </c>
+      <c r="N664" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="665" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A665" t="s">
+        <v>3563</v>
+      </c>
+      <c r="B665" t="s">
+        <v>3564</v>
+      </c>
+      <c r="E665" t="s">
+        <v>3565</v>
+      </c>
+      <c r="F665" t="s">
+        <v>9</v>
+      </c>
+      <c r="G665" t="s">
+        <v>3565</v>
+      </c>
+      <c r="H665" t="s">
+        <v>9</v>
+      </c>
+      <c r="I665">
+        <v>13.75604</v>
+      </c>
+      <c r="J665">
+        <v>100.50526000000001</v>
+      </c>
+      <c r="M665" t="s">
+        <v>3566</v>
+      </c>
+      <c r="N665" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="666" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A666" t="s">
+        <v>3567</v>
+      </c>
+      <c r="B666" t="s">
+        <v>3568</v>
+      </c>
+      <c r="E666" t="s">
+        <v>3569</v>
+      </c>
+      <c r="F666" t="s">
+        <v>9</v>
+      </c>
+      <c r="G666" t="s">
+        <v>3569</v>
+      </c>
+      <c r="H666" t="s">
+        <v>9</v>
+      </c>
+      <c r="I666">
+        <v>13.74827</v>
+      </c>
+      <c r="J666">
+        <v>100.56929</v>
+      </c>
+      <c r="M666" t="s">
+        <v>3570</v>
+      </c>
+      <c r="N666" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="667" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A667" t="s">
+        <v>3571</v>
+      </c>
+      <c r="E667" t="s">
+        <v>943</v>
+      </c>
+      <c r="F667" t="s">
+        <v>9</v>
+      </c>
+      <c r="G667" t="s">
+        <v>9</v>
+      </c>
+      <c r="H667" t="s">
+        <v>9</v>
+      </c>
+      <c r="I667">
+        <v>13.67304</v>
+      </c>
+      <c r="J667">
+        <v>100.6065</v>
+      </c>
+      <c r="M667" t="s">
+        <v>3572</v>
+      </c>
+      <c r="N667" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="668" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A668" t="s">
+        <v>3573</v>
+      </c>
+      <c r="E668" t="s">
+        <v>943</v>
+      </c>
+      <c r="F668" t="s">
+        <v>9</v>
+      </c>
+      <c r="G668" t="s">
+        <v>9</v>
+      </c>
+      <c r="H668" t="s">
+        <v>9</v>
+      </c>
+      <c r="I668">
+        <v>13.6729</v>
+      </c>
+      <c r="J668">
+        <v>100.60681</v>
+      </c>
+      <c r="M668" t="s">
+        <v>3574</v>
+      </c>
+      <c r="N668" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="669" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A669" t="s">
+        <v>3575</v>
+      </c>
+      <c r="E669" t="s">
+        <v>3576</v>
+      </c>
+      <c r="F669" t="s">
+        <v>9</v>
+      </c>
+      <c r="G669" t="s">
+        <v>3576</v>
+      </c>
+      <c r="H669" t="s">
+        <v>9</v>
+      </c>
+      <c r="I669">
+        <v>13.67266</v>
+      </c>
+      <c r="J669">
+        <v>100.45635</v>
+      </c>
+      <c r="M669" t="s">
+        <v>3577</v>
+      </c>
+      <c r="N669" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="670" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A670" t="s">
+        <v>3578</v>
+      </c>
+      <c r="E670" t="s">
+        <v>3579</v>
+      </c>
+      <c r="F670" t="s">
+        <v>9</v>
+      </c>
+      <c r="G670" t="s">
+        <v>3579</v>
+      </c>
+      <c r="H670" t="s">
+        <v>9</v>
+      </c>
+      <c r="I670">
+        <v>13.85751</v>
+      </c>
+      <c r="J670">
+        <v>100.62732</v>
+      </c>
+      <c r="M670" t="s">
+        <v>3580</v>
+      </c>
+      <c r="N670" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="671" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A671" t="s">
+        <v>3581</v>
+      </c>
+      <c r="E671" t="s">
+        <v>3582</v>
+      </c>
+      <c r="F671" t="s">
+        <v>9</v>
+      </c>
+      <c r="G671" t="s">
+        <v>9</v>
+      </c>
+      <c r="H671" t="s">
+        <v>9</v>
+      </c>
+      <c r="I671">
+        <v>13.95072</v>
+      </c>
+      <c r="J671">
+        <v>100.62215999999999</v>
+      </c>
+      <c r="M671" t="s">
+        <v>3583</v>
+      </c>
+      <c r="N671" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="672" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A672" t="s">
+        <v>3584</v>
+      </c>
+      <c r="E672" t="s">
+        <v>3585</v>
+      </c>
+      <c r="F672" t="s">
+        <v>9</v>
+      </c>
+      <c r="G672" t="s">
+        <v>3585</v>
+      </c>
+      <c r="H672" t="s">
+        <v>9</v>
+      </c>
+      <c r="I672">
+        <v>13.765930000000001</v>
+      </c>
+      <c r="J672">
+        <v>100.48764</v>
+      </c>
+      <c r="M672" t="s">
+        <v>3586</v>
+      </c>
+      <c r="N672" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="673" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A673" t="s">
+        <v>3587</v>
+      </c>
+      <c r="E673" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F673" t="s">
+        <v>9</v>
+      </c>
+      <c r="G673" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H673" t="s">
+        <v>9</v>
+      </c>
+      <c r="I673">
+        <v>13.76769</v>
+      </c>
+      <c r="J673">
+        <v>100.48497</v>
+      </c>
+      <c r="M673" t="s">
+        <v>3588</v>
+      </c>
+      <c r="N673" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="674" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A674" t="s">
+        <v>3589</v>
+      </c>
+      <c r="E674" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F674" t="s">
+        <v>9</v>
+      </c>
+      <c r="G674" t="s">
+        <v>3590</v>
+      </c>
+      <c r="H674" t="s">
+        <v>9</v>
+      </c>
+      <c r="I674">
+        <v>13.76605</v>
+      </c>
+      <c r="J674">
+        <v>100.48784000000001</v>
+      </c>
+      <c r="M674" t="s">
+        <v>3591</v>
+      </c>
+      <c r="N674" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="675" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A675" t="s">
+        <v>3592</v>
+      </c>
+      <c r="E675" t="s">
+        <v>3593</v>
+      </c>
+      <c r="F675" t="s">
+        <v>3594</v>
+      </c>
+      <c r="G675" t="s">
+        <v>3595</v>
+      </c>
+      <c r="H675" t="s">
+        <v>3596</v>
+      </c>
+      <c r="I675">
+        <v>13.75318</v>
+      </c>
+      <c r="J675">
+        <v>100.49848</v>
+      </c>
+      <c r="M675" t="s">
+        <v>3597</v>
+      </c>
+      <c r="N675" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="676" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A676" t="s">
+        <v>3598</v>
+      </c>
+      <c r="E676" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F676" t="s">
+        <v>9</v>
+      </c>
+      <c r="G676" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H676" t="s">
+        <v>9</v>
+      </c>
+      <c r="I676">
+        <v>13.769410000000001</v>
+      </c>
+      <c r="J676">
+        <v>100.50355</v>
+      </c>
+      <c r="M676" t="s">
+        <v>3599</v>
+      </c>
+      <c r="N676" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="677" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A677" t="s">
+        <v>3600</v>
+      </c>
+      <c r="E677" t="s">
+        <v>3601</v>
+      </c>
+      <c r="F677" t="s">
+        <v>3602</v>
+      </c>
+      <c r="G677" t="s">
+        <v>3603</v>
+      </c>
+      <c r="H677" t="s">
+        <v>3604</v>
+      </c>
+      <c r="I677">
+        <v>13.740180000000001</v>
+      </c>
+      <c r="J677">
+        <v>100.49791999999999</v>
+      </c>
+      <c r="M677" t="s">
+        <v>3605</v>
+      </c>
+      <c r="N677" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="678" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A678" t="s">
+        <v>3606</v>
+      </c>
+      <c r="E678" t="s">
+        <v>3607</v>
+      </c>
+      <c r="F678" t="s">
+        <v>9</v>
+      </c>
+      <c r="G678" t="s">
+        <v>3608</v>
+      </c>
+      <c r="H678" t="s">
+        <v>9</v>
+      </c>
+      <c r="I678">
+        <v>13.75736</v>
+      </c>
+      <c r="J678">
+        <v>100.49906</v>
+      </c>
+      <c r="M678" t="s">
+        <v>3609</v>
+      </c>
+      <c r="N678" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="679" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A679" t="s">
+        <v>3610</v>
+      </c>
+      <c r="E679" t="s">
+        <v>338</v>
+      </c>
+      <c r="F679" t="s">
+        <v>9</v>
+      </c>
+      <c r="G679" t="s">
+        <v>338</v>
+      </c>
+      <c r="H679" t="s">
+        <v>9</v>
+      </c>
+      <c r="I679">
+        <v>13.760009999999999</v>
+      </c>
+      <c r="J679">
+        <v>100.5077</v>
+      </c>
+      <c r="M679" t="s">
+        <v>3611</v>
+      </c>
+      <c r="N679" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="680" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A680" t="s">
+        <v>3612</v>
+      </c>
+      <c r="E680" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F680" t="s">
+        <v>9</v>
+      </c>
+      <c r="G680" t="s">
+        <v>1198</v>
+      </c>
+      <c r="H680" t="s">
+        <v>9</v>
+      </c>
+      <c r="I680">
+        <v>13.74403</v>
+      </c>
+      <c r="J680">
+        <v>100.54391</v>
+      </c>
+      <c r="M680" t="s">
+        <v>3613</v>
+      </c>
+      <c r="N680" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="681" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A681" t="s">
+        <v>3614</v>
+      </c>
+      <c r="E681" t="s">
+        <v>3615</v>
+      </c>
+      <c r="F681" t="s">
+        <v>128</v>
+      </c>
+      <c r="G681" t="s">
+        <v>3616</v>
+      </c>
+      <c r="H681" t="s">
+        <v>3617</v>
+      </c>
+      <c r="I681">
+        <v>13.77342</v>
+      </c>
+      <c r="J681">
+        <v>100.482</v>
+      </c>
+      <c r="M681" t="s">
+        <v>3618</v>
+      </c>
+      <c r="N681" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="682" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A682" t="s">
+        <v>3619</v>
+      </c>
+      <c r="E682" t="s">
+        <v>3620</v>
+      </c>
+      <c r="F682" t="s">
+        <v>1518</v>
+      </c>
+      <c r="G682" t="s">
+        <v>3621</v>
+      </c>
+      <c r="H682" t="s">
+        <v>3622</v>
+      </c>
+      <c r="I682">
+        <v>13.76258</v>
+      </c>
+      <c r="J682">
+        <v>100.50439</v>
+      </c>
+      <c r="M682" t="s">
+        <v>3623</v>
+      </c>
+      <c r="N682" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="683" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A683" t="s">
+        <v>3624</v>
+      </c>
+      <c r="E683" t="s">
+        <v>328</v>
+      </c>
+      <c r="F683" t="s">
+        <v>9</v>
+      </c>
+      <c r="G683" t="s">
+        <v>328</v>
+      </c>
+      <c r="H683" t="s">
+        <v>9</v>
+      </c>
+      <c r="I683">
+        <v>13.75179</v>
+      </c>
+      <c r="J683">
+        <v>100.50045</v>
+      </c>
+      <c r="M683" t="s">
+        <v>3625</v>
+      </c>
+      <c r="N683" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="684" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A684" t="s">
+        <v>3626</v>
+      </c>
+      <c r="E684" t="s">
+        <v>1934</v>
+      </c>
+      <c r="F684" t="s">
+        <v>1761</v>
+      </c>
+      <c r="G684" t="s">
+        <v>3627</v>
+      </c>
+      <c r="H684" t="s">
+        <v>3628</v>
+      </c>
+      <c r="I684">
+        <v>13.712669999999999</v>
+      </c>
+      <c r="J684">
+        <v>100.48844</v>
+      </c>
+      <c r="M684" t="s">
+        <v>3629</v>
+      </c>
+      <c r="N684" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="685" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A685" t="s">
+        <v>3630</v>
+      </c>
+      <c r="E685" t="s">
+        <v>3631</v>
+      </c>
+      <c r="F685" t="s">
+        <v>3632</v>
+      </c>
+      <c r="G685" t="s">
+        <v>3633</v>
+      </c>
+      <c r="H685" t="s">
+        <v>3634</v>
+      </c>
+      <c r="I685">
+        <v>13.74709</v>
+      </c>
+      <c r="J685">
+        <v>100.50944</v>
+      </c>
+      <c r="M685" t="s">
+        <v>3635</v>
+      </c>
+      <c r="N685" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="686" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A686" t="s">
+        <v>3636</v>
+      </c>
+      <c r="E686" t="s">
+        <v>3637</v>
+      </c>
+      <c r="F686" t="s">
+        <v>3638</v>
+      </c>
+      <c r="G686" t="s">
+        <v>3639</v>
+      </c>
+      <c r="H686" t="s">
+        <v>3640</v>
+      </c>
+      <c r="I686">
+        <v>13.749280000000001</v>
+      </c>
+      <c r="J686">
+        <v>100.50754000000001</v>
+      </c>
+      <c r="M686" t="s">
+        <v>3641</v>
+      </c>
+      <c r="N686" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>